<commit_message>
new changes in latency
</commit_message>
<xml_diff>
--- a/Latency_ddata.xlsx
+++ b/Latency_ddata.xlsx
@@ -386,7 +386,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -411,206 +411,19 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2">
-        <v>0.4737546866630959</v>
+        <v>0.5496434448710916</v>
       </c>
       <c r="B2">
-        <v>1689837819.330059</v>
+        <v>1689839664.873628</v>
       </c>
       <c r="C2">
-        <v>0.8267007723325372</v>
+        <v>0.9767541235291549</v>
       </c>
       <c r="D2">
-        <v>1689837819.479659</v>
+        <v>1689839664.992314</v>
       </c>
       <c r="E2">
-        <v>0.1495997905731201</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3">
-        <v>0.2878950187466524</v>
-      </c>
-      <c r="B3">
-        <v>1689837824.316724</v>
-      </c>
-      <c r="C3">
-        <v>0.7390704201391858</v>
-      </c>
-      <c r="D3">
-        <v>1689837824.469316</v>
-      </c>
-      <c r="E3">
-        <v>0.1525917053222656</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4">
-        <v>0.5865024102838778</v>
-      </c>
-      <c r="B4">
-        <v>1689837829.331314</v>
-      </c>
-      <c r="C4">
-        <v>0.4815092994472783</v>
-      </c>
-      <c r="D4">
-        <v>1689837829.469943</v>
-      </c>
-      <c r="E4">
-        <v>0.1386291980743408</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5">
-        <v>0.450187466523835</v>
-      </c>
-      <c r="B5">
-        <v>1689837834.309997</v>
-      </c>
-      <c r="C5">
-        <v>0.2142855909642813</v>
-      </c>
-      <c r="D5">
-        <v>1689837834.4596</v>
-      </c>
-      <c r="E5">
-        <v>0.1496028900146484</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6">
-        <v>0.2905731119442956</v>
-      </c>
-      <c r="B6">
-        <v>1689837839.31162</v>
-      </c>
-      <c r="C6">
-        <v>0.908681786126467</v>
-      </c>
-      <c r="D6">
-        <v>1689837839.469205</v>
-      </c>
-      <c r="E6">
-        <v>0.1575846672058105</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7">
-        <v>0.5838243170862346</v>
-      </c>
-      <c r="B7">
-        <v>1689837844.326246</v>
-      </c>
-      <c r="C7">
-        <v>0.6561312563614333</v>
-      </c>
-      <c r="D7">
-        <v>1689837844.469826</v>
-      </c>
-      <c r="E7">
-        <v>0.1435801982879639</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8">
-        <v>0.463310123192287</v>
-      </c>
-      <c r="B8">
-        <v>1689837849.325842</v>
-      </c>
-      <c r="C8">
-        <v>0.3926773032115088</v>
-      </c>
-      <c r="D8">
-        <v>1689837849.45952</v>
-      </c>
-      <c r="E8">
-        <v>0.1336774826049805</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9">
-        <v>0.30878414568827</v>
-      </c>
-      <c r="B9">
-        <v>1689837854.320483</v>
-      </c>
-      <c r="C9">
-        <v>0.9623870451722627</v>
-      </c>
-      <c r="D9">
-        <v>1689837854.470082</v>
-      </c>
-      <c r="E9">
-        <v>0.149599552154541</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10">
-        <v>0.5549009105516872</v>
-      </c>
-      <c r="B10">
-        <v>1689837859.311137</v>
-      </c>
-      <c r="C10">
-        <v>0.7274398524786267</v>
-      </c>
-      <c r="D10">
-        <v>1689837859.469711</v>
-      </c>
-      <c r="E10">
-        <v>0.1585736274719238</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11">
-        <v>0.4528655597214783</v>
-      </c>
-      <c r="B11">
-        <v>1689837864.318745</v>
-      </c>
-      <c r="C11">
-        <v>0.5131842450654038</v>
-      </c>
-      <c r="D11">
-        <v>1689837864.459368</v>
-      </c>
-      <c r="E11">
-        <v>0.1406235694885254</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12">
-        <v>0.2932512051419389</v>
-      </c>
-      <c r="B12">
-        <v>1689837869.305406</v>
-      </c>
-      <c r="C12">
-        <v>0.221861415681708</v>
-      </c>
-      <c r="D12">
-        <v>1689837869.449023</v>
-      </c>
-      <c r="E12">
-        <v>0.1436173915863037</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13">
-        <v>0.5707016604177826</v>
-      </c>
-      <c r="B13">
-        <v>1689837874.321009</v>
-      </c>
-      <c r="C13">
-        <v>0.7428583037228981</v>
-      </c>
-      <c r="D13">
-        <v>1689837874.469615</v>
-      </c>
-      <c r="E13">
-        <v>0.1486058235168457</v>
+        <v>0.1186857223510742</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new changes in latency_1
</commit_message>
<xml_diff>
--- a/Latency_ddata.xlsx
+++ b/Latency_ddata.xlsx
@@ -386,7 +386,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -411,19 +411,206 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2">
-        <v>0.5496434448710916</v>
+        <v>0.1485482781904119</v>
       </c>
       <c r="B2">
-        <v>1689839664.873628</v>
+        <v>1689843629.714195</v>
       </c>
       <c r="C2">
-        <v>0.9767541235291549</v>
+        <v>0.3743307501007689</v>
       </c>
       <c r="D2">
-        <v>1689839664.992314</v>
+        <v>1689843629.799342</v>
       </c>
       <c r="E2">
-        <v>0.1186857223510742</v>
+        <v>0.08514714241027832</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>0.08912896691424713</v>
+      </c>
+      <c r="B3">
+        <v>1689843634.716197</v>
+      </c>
+      <c r="C3">
+        <v>0.06667587402748519</v>
+      </c>
+      <c r="D3">
+        <v>1689843634.800273</v>
+      </c>
+      <c r="E3">
+        <v>0.0840761661529541</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>0.03308575286968264</v>
+      </c>
+      <c r="B4">
+        <v>1689843639.701746</v>
+      </c>
+      <c r="C4">
+        <v>0.7917310801664017</v>
+      </c>
+      <c r="D4">
+        <v>1689843639.808546</v>
+      </c>
+      <c r="E4">
+        <v>0.1067993640899658</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>0.224510465901418</v>
+      </c>
+      <c r="B5">
+        <v>1689843644.717801</v>
+      </c>
+      <c r="C5">
+        <v>0.5067153602202465</v>
+      </c>
+      <c r="D5">
+        <v>1689843644.799302</v>
+      </c>
+      <c r="E5">
+        <v>0.08150076866149902</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>0.1583389601620526</v>
+      </c>
+      <c r="B6">
+        <v>1689843649.719811</v>
+      </c>
+      <c r="C6">
+        <v>0.2526672193111211</v>
+      </c>
+      <c r="D6">
+        <v>1689843649.798629</v>
+      </c>
+      <c r="E6">
+        <v>0.07881784439086914</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>0.1056718433490885</v>
+      </c>
+      <c r="B7">
+        <v>1689843654.715734</v>
+      </c>
+      <c r="C7">
+        <v>0.01247903626919362</v>
+      </c>
+      <c r="D7">
+        <v>1689843653.838972</v>
+      </c>
+      <c r="E7">
+        <v>0.8767616748809814</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>0.0462525320729237</v>
+      </c>
+      <c r="B8">
+        <v>1689843659.718307</v>
+      </c>
+      <c r="C8">
+        <v>0.01249728874658717</v>
+      </c>
+      <c r="D8">
+        <v>1689843659.248995</v>
+      </c>
+      <c r="E8">
+        <v>0.4693119525909424</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9">
+        <v>0.2045914922349764</v>
+      </c>
+      <c r="B9">
+        <v>1689843664.715051</v>
+      </c>
+      <c r="C9">
+        <v>0.4027382366585798</v>
+      </c>
+      <c r="D9">
+        <v>1689843664.798724</v>
+      </c>
+      <c r="E9">
+        <v>0.08367323875427246</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10">
+        <v>0.1451721809588116</v>
+      </c>
+      <c r="B10">
+        <v>1689843669.713756</v>
+      </c>
+      <c r="C10">
+        <v>0.01267664975777441</v>
+      </c>
+      <c r="D10">
+        <v>1689843668.979332</v>
+      </c>
+      <c r="E10">
+        <v>0.7344245910644531</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11">
+        <v>0.08575286968264685</v>
+      </c>
+      <c r="B11">
+        <v>1689843674.696821</v>
+      </c>
+      <c r="C11">
+        <v>0.0125041638464054</v>
+      </c>
+      <c r="D11">
+        <v>1689843672.778796</v>
+      </c>
+      <c r="E11">
+        <v>1.918024778366089</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12">
+        <v>0.08575286968264685</v>
+      </c>
+      <c r="B12">
+        <v>1689843674.696821</v>
+      </c>
+      <c r="C12">
+        <v>0.02056579637840428</v>
+      </c>
+      <c r="D12">
+        <v>1689843675.785807</v>
+      </c>
+      <c r="E12">
+        <v>1.088986396789551</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13">
+        <v>0.02295746117488183</v>
+      </c>
+      <c r="B13">
+        <v>1689843679.6954</v>
+      </c>
+      <c r="C13">
+        <v>0.5741404984447368</v>
+      </c>
+      <c r="D13">
+        <v>1689843679.800069</v>
+      </c>
+      <c r="E13">
+        <v>0.1046686172485352</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Code completion for demo 3
</commit_message>
<xml_diff>
--- a/Latency_ddata.xlsx
+++ b/Latency_ddata.xlsx
@@ -411,206 +411,206 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2">
-        <v>0.7754581303641847</v>
+        <v>0.6117092866756392</v>
       </c>
       <c r="B2">
-        <v>1689923302.067704</v>
+        <v>1690369242.192249</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0.9700400031215803</v>
       </c>
       <c r="D2">
-        <v>1689923302.104089</v>
+        <v>1690369242.259881</v>
       </c>
       <c r="E2">
-        <v>0.03638529777526855</v>
+        <v>0.06763243675231934</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3">
-        <v>0.356065877986546</v>
+        <v>0.2893674293405114</v>
       </c>
       <c r="B3">
-        <v>1689923307.047287</v>
+        <v>1690369247.180922</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>0.7457110641474254</v>
       </c>
       <c r="D3">
-        <v>1689923307.094062</v>
+        <v>1690369247.249108</v>
       </c>
       <c r="E3">
-        <v>0.04677438735961914</v>
+        <v>0.06818628311157227</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4">
-        <v>0.8095569473440037</v>
+        <v>0.4703903095558546</v>
       </c>
       <c r="B4">
-        <v>1689923312.06251</v>
+        <v>1690369252.184102</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>0.5088808143078496</v>
       </c>
       <c r="D4">
-        <v>1689923312.09407</v>
+        <v>1690369252.240347</v>
       </c>
       <c r="E4">
-        <v>0.03156089782714844</v>
+        <v>0.05624556541442871</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5">
-        <v>0.7754581303641847</v>
+        <v>0.6117092866756392</v>
       </c>
       <c r="B5">
-        <v>1689923317.056996</v>
+        <v>1690369257.198658</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>0.2640038046884596</v>
       </c>
       <c r="D5">
-        <v>1689923317.103748</v>
+        <v>1690369257.239956</v>
       </c>
       <c r="E5">
-        <v>0.04675197601318359</v>
+        <v>0.04129815101623535</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6">
-        <v>0.714219438645326</v>
+        <v>0.4966352624495289</v>
       </c>
       <c r="B6">
-        <v>1689923322.04762</v>
+        <v>1690369262.184294</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>0.9556950817962525</v>
       </c>
       <c r="D6">
-        <v>1689923322.093939</v>
+        <v>1690369262.24972</v>
       </c>
       <c r="E6">
-        <v>0.04631900787353516</v>
+        <v>0.06542539596557617</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7">
-        <v>0.2289491997216423</v>
+        <v>0.4175639300134589</v>
       </c>
       <c r="B7">
-        <v>1689923327.040141</v>
+        <v>1690369267.17212</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>0.7199734245730661</v>
       </c>
       <c r="D7">
-        <v>1689923327.094142</v>
+        <v>1690369267.240569</v>
       </c>
       <c r="E7">
-        <v>0.0540013313293457</v>
+        <v>0.06844902038574219</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8">
-        <v>0.5395499884017629</v>
+        <v>0.3024899057873485</v>
       </c>
       <c r="B8">
-        <v>1689923332.042604</v>
+        <v>1690369272.17943</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>0.4483742410832863</v>
       </c>
       <c r="D8">
-        <v>1689923332.104177</v>
+        <v>1690369272.239869</v>
       </c>
       <c r="E8">
-        <v>0.06157374382019043</v>
+        <v>0.06043910980224609</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9">
-        <v>0.7323126884713523</v>
+        <v>0.4801480484522207</v>
       </c>
       <c r="B9">
-        <v>1689923337.0628</v>
+        <v>1690369277.203125</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>0.1872779038191648</v>
       </c>
       <c r="D9">
-        <v>1689923337.094167</v>
+        <v>1690369277.229915</v>
       </c>
       <c r="E9">
-        <v>0.03136730194091797</v>
+        <v>0.02678990364074707</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10">
-        <v>0.6372071445140339</v>
+        <v>0.595222072678331</v>
       </c>
       <c r="B10">
-        <v>1689923342.041045</v>
+        <v>1690369282.192439</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>0.9001615732764729</v>
       </c>
       <c r="D10">
-        <v>1689923342.093565</v>
+        <v>1690369282.239987</v>
       </c>
       <c r="E10">
-        <v>0.052520751953125</v>
+        <v>0.04754829406738281</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11">
-        <v>0.5395499884017629</v>
+        <v>0.5262449528936743</v>
       </c>
       <c r="B11">
-        <v>1689923347.048923</v>
+        <v>1690369287.1872</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>0.5847835091905227</v>
       </c>
       <c r="D11">
-        <v>1689923347.104055</v>
+        <v>1690369287.239927</v>
       </c>
       <c r="E11">
-        <v>0.05513119697570801</v>
+        <v>0.05272698402404785</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12">
-        <v>0.3718394803989793</v>
+        <v>0.4407806191117093</v>
       </c>
       <c r="B12">
-        <v>1689923352.045</v>
+        <v>1690369292.191486</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>0.3247972226800773</v>
       </c>
       <c r="D12">
-        <v>1689923352.094053</v>
+        <v>1690369292.229494</v>
       </c>
       <c r="E12">
-        <v>0.04905247688293457</v>
+        <v>0.03800797462463379</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13">
-        <v>0.6599396891672465</v>
+        <v>0.335464333781965</v>
       </c>
       <c r="B13">
-        <v>1689923357.048815</v>
+        <v>1690369297.183312</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>0.9859821680308416</v>
       </c>
       <c r="D13">
-        <v>1689923357.093524</v>
+        <v>1690369297.240759</v>
       </c>
       <c r="E13">
-        <v>0.04470920562744141</v>
+        <v>0.05744743347167969</v>
       </c>
     </row>
   </sheetData>

</xml_diff>